<commit_message>
Move selection and better generation
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -78,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +105,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -137,12 +149,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -427,7 +442,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,13 +463,13 @@
       <c r="D1">
         <v>59</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="7">
         <v>60</v>
       </c>
       <c r="F1">
         <v>61</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="7">
         <v>62</v>
       </c>
       <c r="H1">
@@ -503,7 +518,7 @@
       <c r="C2">
         <v>50</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="7">
         <v>51</v>
       </c>
       <c r="E2">
@@ -515,7 +530,7 @@
       <c r="G2">
         <v>54</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="7">
         <v>55</v>
       </c>
       <c r="I2" s="1">
@@ -567,16 +582,16 @@
       <c r="C3">
         <v>42</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>43</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <v>44</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="5">
         <v>45</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="6">
         <v>46</v>
       </c>
       <c r="H3">
@@ -628,22 +643,22 @@
       <c r="B4">
         <v>33</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>34</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="7">
         <v>35</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>36</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="6">
         <v>37</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="6">
         <v>38</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="7">
         <v>39</v>
       </c>
       <c r="I4" s="1">
@@ -692,22 +707,22 @@
       <c r="B5">
         <v>25</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="6">
         <v>26</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>27</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="7">
         <v>28</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="6">
         <v>29</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="7">
         <v>30</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="6">
         <v>31</v>
       </c>
       <c r="I5" s="1">
@@ -756,22 +771,22 @@
       <c r="B6">
         <v>17</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>18</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>19</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>20</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>21</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <v>22</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="6">
         <v>23</v>
       </c>
       <c r="I6" s="1">
@@ -823,19 +838,19 @@
       <c r="C7">
         <v>10</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>11</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>12</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <v>13</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <v>14</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <v>15</v>
       </c>
       <c r="I7" s="1">

</xml_diff>